<commit_message>
Added some notes for 2022 global study, missing findings and future work, still need to read past bm ratio into global variations
</commit_message>
<xml_diff>
--- a/Lit Review.xlsx
+++ b/Lit Review.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varunchodanker/Documents/UoB_Uni_Work/Individual Project/PROJECT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varunchodanker/Documents/UoB_Uni_Work/Individual Project/PROJECT/MSc-Individual-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89227C6-8112-0348-8C42-139878329A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E56723-9499-C746-B1B4-5D0526C8707B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{240C8A50-B89B-4C88-924D-AD3AB59AF65A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>ID Number</t>
   </si>
@@ -182,24 +182,54 @@
 countries with lower economic development, larger energy sectors, and less inclusive political systems. Premia related to emission levels are higher in countries with stricter domestic climate policies. The latter have increased with investor awareness about climate change risk.</t>
   </si>
   <si>
-    <t>Return on equity,
-Sales growth,
-YoY emissions change,
-Raw emissions level,</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Note, as stated in the paper, the 
 features are lagged compared 
 to the dependent variable, which 
 is equity return.</t>
   </si>
   <si>
+    <t>Model and determine the pricing 
+of carbon emissions, broken 
+down into scopes 1,2 and 3, in the global equity environment (where carbon emissions data is available).
+Then, explore the variance in the premiums due to geographic region. Consider aspects such as politics, energy mix and technology.</t>
+  </si>
+  <si>
+    <t>Trucost for emissions data.</t>
+  </si>
+  <si>
+    <t>Firm characteristics-based approach as opposed to a risk-based approach. Therefore, entailed the discovery of a carbon beta as opposed to a carbon alpha, w.r.t mispricing. 
+Based on classic econometrics</t>
+  </si>
+  <si>
     <t>Controlled for earnings growth 
 through:
 - sales growth
 - return on equity
-[not sure if I should do this]
-Controlled for fixed effects</t>
+-&gt; sales revenue could drive emissions &amp; returns, thus accounted for size to ensure the distinct relationships are captured
+Controlled for fixed effects
+- country, year-month, industry
+Controlled for many firm characteristics
+Log versions of many variables
+Double clustered standard error by the firm and year</t>
+  </si>
+  <si>
+    <t>Monthy returns, annual returns, book to market ratio
+Absolute carbon emission levels,
+Growth in carbon emission levels (winsorized),
+- low correlation
+Return on equity,
+Sales growth,
+YoY emissions change,
+Raw emissions level,
+Country, year month &amp; industry fixed effects</t>
+  </si>
+  <si>
+    <t>Returns are noisy, backup test for 
+expected return could be useful
+Carbon beta vs carbon alpha
+- fixed effects, firm features
+Breakdown of carbon emission scopes
+Consideration of short-term/transitory component of transition risk (variable)</t>
   </si>
 </sst>
 </file>
@@ -602,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58E4A02-4BAA-41E0-832C-5DABBFDCD6F8}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="181" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="M3" zoomScale="181" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -712,7 +742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="208" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" ht="260" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -728,14 +758,26 @@
       <c r="G3" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="I3" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="J3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="L3" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="M3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="P3" s="5" t="s">
-        <v>34</v>
+      <c r="Q3" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some more details to 2022 global on applicability and controls
</commit_message>
<xml_diff>
--- a/Lit Review.xlsx
+++ b/Lit Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varunchodanker/Documents/UoB_Uni_Work/Individual Project/PROJECT/MSc-Individual-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E56723-9499-C746-B1B4-5D0526C8707B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27B01C4-486D-DC4F-884F-FF5E97623733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{240C8A50-B89B-4C88-924D-AD3AB59AF65A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>ID Number</t>
   </si>
@@ -224,12 +224,21 @@
 Country, year month &amp; industry fixed effects</t>
   </si>
   <si>
+    <t>Carbon emissions levels are a 
+persistent characteristic when 
+the news effect is taken 
+out
+- backwards imputing emissions leads to similar premia</t>
+  </si>
+  <si>
     <t>Returns are noisy, backup test for 
 expected return could be useful
 Carbon beta vs carbon alpha
 - fixed effects, firm features
 Breakdown of carbon emission scopes
-Consideration of short-term/transitory component of transition risk (variable)</t>
+Consideration of short-term/transitory component of transition risk (variable)
+There are horizon effects to consider when modelling
+Information effects analyses of Trucost are likely (almost directly) applicable in my case</t>
   </si>
 </sst>
 </file>
@@ -632,7 +641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58E4A02-4BAA-41E0-832C-5DABBFDCD6F8}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M3" zoomScale="181" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M2" zoomScale="181" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
@@ -773,11 +782,14 @@
       <c r="M3" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="N3" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="P3" s="5" t="s">
         <v>33</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added findings from 2022 JoF global study, mainly w.r.t country-level metric variations, also filled keywords, location, journal
</commit_message>
<xml_diff>
--- a/Lit Review.xlsx
+++ b/Lit Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varunchodanker/Documents/UoB_Uni_Work/Individual Project/PROJECT/MSc-Individual-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27B01C4-486D-DC4F-884F-FF5E97623733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DF43E1-1DE6-6843-97EF-8E03FD62E2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{240C8A50-B89B-4C88-924D-AD3AB59AF65A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>ID Number</t>
   </si>
@@ -173,9 +173,6 @@
 Marcin Kacperczyk;
 2022;
 Global Pricing of Carbon-Transition Risk</t>
-  </si>
-  <si>
-    <t>Journal of Finance forthcoming</t>
   </si>
   <si>
     <t>The energy transition away from fossil fuels exposes companies to carbon-transition risk. Estimating the market-based premium associated with carbon-transition risk in a cross-section of 14,400 firms in 77 countries, we find higher stock returns associated with higher levels and growth rates of carbon emissions in all sectors and most countries. Carbon premia related to emissions growth are greater for firms located in
@@ -224,13 +221,6 @@
 Country, year month &amp; industry fixed effects</t>
   </si>
   <si>
-    <t>Carbon emissions levels are a 
-persistent characteristic when 
-the news effect is taken 
-out
-- backwards imputing emissions leads to similar premia</t>
-  </si>
-  <si>
     <t>Returns are noisy, backup test for 
 expected return could be useful
 Carbon beta vs carbon alpha
@@ -240,12 +230,63 @@
 There are horizon effects to consider when modelling
 Information effects analyses of Trucost are likely (almost directly) applicable in my case</t>
   </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/10.1111/jofi.13272</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/10.1111/jifm.12190</t>
+  </si>
+  <si>
+    <t>BOLTON, P. and 
+KACPERCZYK, M. (2023), Global Pricing of Carbon-Transition Risk. J Finance, 78: 3677-3754. https://doi.org/10.1111/jofi.13272</t>
+  </si>
+  <si>
+    <t>Generalised global transition risk premium exists in the equity markets, but this varies across countries based on different characteristics.
+- w.r.t both short-term and long-term transition risk
+Carbon emissions levels are a 
+persistent characteristic when 
+the news effect is taken 
+out
+- backwards imputing emissions leads to similar premia
+Energy mix (renewable&amp;fossil fuel share) influences premium magnitudes but consumption does not
+- demonstrated by the (significant) interaction terms
+Sociopolitical environment affects premium, transitory shock
+- rule of law: -ve
+- voice: -ve
+- gini ineq: +ve
+Climate policy tightness
+- seen as permanent shock
+Brown reputation risk
+- 'baked in'?
+Physical risk, insignificant interactions w transition risk
+Investor concern (discount rate channel)
+- level not growth
+- change in long term beliefs
+- robust: international policy -&gt; national policy
+Green equilibrium
+- repricing
+Potential underestimation of 
+carbon risk premium</t>
+  </si>
+  <si>
+    <t>Korea, Carbon, Risk, Pricing, 
+Stock, Emissions, Emerging, Markets, Cross-sectional, Association, Foreign, Ownership</t>
+  </si>
+  <si>
+    <t>Global, Pricing, Transition, 
+Risk, Carbon, Cross-sectional, 
+Markets, Countries, Emissions, 
+Short-term, Long-term, Risk</t>
+  </si>
+  <si>
+    <t>Journal of Finance [4*]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +305,14 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -307,10 +356,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -325,8 +375,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -641,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58E4A02-4BAA-41E0-832C-5DABBFDCD6F8}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M2" zoomScale="181" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="181" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -722,8 +776,14 @@
       <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="F2" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="G2" s="5" t="s">
         <v>21</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>29</v>
@@ -751,7 +811,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="260" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -759,40 +819,53 @@
         <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>45</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="F3" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="G3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{5409ACC0-6A7D-FC46-A2E2-B0315444F1EA}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{14301C01-51B3-954A-9C1A-AB865D523541}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed keywords + new src
</commit_message>
<xml_diff>
--- a/Lit Review.xlsx
+++ b/Lit Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varunchodanker/Documents/UoB_Uni_Work/Individual Project/PROJECT/MSc-Individual-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DF43E1-1DE6-6843-97EF-8E03FD62E2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F4A404-0B7B-F043-BBA1-CF2DC0A93E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{240C8A50-B89B-4C88-924D-AD3AB59AF65A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>ID Number</t>
   </si>
@@ -269,17 +269,49 @@
 carbon risk premium</t>
   </si>
   <si>
-    <t>Korea, Carbon, Risk, Pricing, 
-Stock, Emissions, Emerging, Markets, Cross-sectional, Association, Foreign, Ownership</t>
-  </si>
-  <si>
-    <t>Global, Pricing, Transition, 
+    <t>Journal of Finance [4*]</t>
+  </si>
+  <si>
+    <t>;
+2020;
+Measuring and Managing Carbon Risk in
+Investment Portfolios</t>
+  </si>
+  <si>
+    <t>This article studies the impact of carbon risk on stock pricing. To address this, we
+consider the seminal approach of G¨orgen et al. (2019), who proposed estimating the
+carbon financial risk of equities by their carbon beta. To achieve this, the primary task
+is to develop a brown-minus-green (or BMG) risk factor, similar to Fama and French
+(1992). Secondly, we must estimate the carbon beta using a multi-factor model. While
+G¨orgen et al. (2019) considered that the carbon beta is constant, we propose a timevarying estimation model to assess the dynamics of the carbon risk. Moreover, we test
+several specifications of the BMG factor to understand which climate change-related
+dimensions are priced in by the stock market. In the second part of the article, we
+focus on the carbon risk management of investment portfolios. First, we analyze how
+carbon risk impacts the construction of a minimum variance portfolio. As the goal of
+this portfolio is to reduce unrewarded financial risks of an investment, incorporating
+the carbon risk into this approach fulfils this objective. Second, we propose a new
+framework for building enhanced index portfolios with a lower exposure to carbon risk
+than capitalization-weighted stock indices. Finally, we explore how carbon sensitivities
+can improve the robustness of factor investing portfolios.</t>
+  </si>
+  <si>
+    <t>Carbon, climate change, risk factor, Kalman filter, minimum variance portfolio,
+enhanced index portfolio, factor investing.</t>
+  </si>
+  <si>
+    <t>carbon risk, empirical asset pricing, Fama-Macbeth regression, GMM</t>
+  </si>
+  <si>
+    <t>N/A: Global, Pricing, Transition, 
 Risk, Carbon, Cross-sectional, 
 Markets, Countries, Emissions, 
 Short-term, Long-term, Risk</t>
   </si>
   <si>
-    <t>Journal of Finance [4*]</t>
+    <t>https://arxiv.org/pdf/2008.13198</t>
+  </si>
+  <si>
+    <t>To fill</t>
   </si>
 </sst>
 </file>
@@ -693,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58E4A02-4BAA-41E0-832C-5DABBFDCD6F8}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="181" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="F5" zoomScale="181" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -777,7 +809,7 @@
         <v>18</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>21</v>
@@ -819,7 +851,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>41</v>
@@ -828,7 +860,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>31</v>
@@ -859,12 +891,33 @@
       </c>
       <c r="Q3" s="5" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="404" x14ac:dyDescent="0.15">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H3" r:id="rId1" xr:uid="{5409ACC0-6A7D-FC46-A2E2-B0315444F1EA}"/>
     <hyperlink ref="H2" r:id="rId2" xr:uid="{14301C01-51B3-954A-9C1A-AB865D523541}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{5C4BD8C1-C1AC-BD42-889B-19C1FF87E844}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added some applicability and objectives from portfolio paper
</commit_message>
<xml_diff>
--- a/Lit Review.xlsx
+++ b/Lit Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varunchodanker/Documents/UoB_Uni_Work/Individual Project/PROJECT/MSc-Individual-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F4A404-0B7B-F043-BBA1-CF2DC0A93E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E47332-ECD8-B743-BD41-AB9D261208BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{240C8A50-B89B-4C88-924D-AD3AB59AF65A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>ID Number</t>
   </si>
@@ -167,12 +167,6 @@
   </si>
   <si>
     <t>Model and test the statistical significance of the relationship between carbon risk and cross-sectional stock returns in the Korean equity market, within the risk-based asset pricing paradigm and while controlling for other traditional return influencing factors. Then, quantify the moderating impact of foreign ownership stake on this relationship.</t>
-  </si>
-  <si>
-    <t>Patrick Bolton, 
-Marcin Kacperczyk;
-2022;
-Global Pricing of Carbon-Transition Risk</t>
   </si>
   <si>
     <t>The energy transition away from fossil fuels exposes companies to carbon-transition risk. Estimating the market-based premium associated with carbon-transition risk in a cross-section of 14,400 firms in 77 countries, we find higher stock returns associated with higher levels and growth rates of carbon emissions in all sectors and most countries. Carbon premia related to emissions growth are greater for firms located in
@@ -311,7 +305,20 @@
     <t>https://arxiv.org/pdf/2008.13198</t>
   </si>
   <si>
-    <t>To fill</t>
+    <t>Patrick Bolton, 
+Marcin Kacperczyk;
+2023;
+Global Pricing of Carbon-Transition Risk</t>
+  </si>
+  <si>
+    <t>Compute the BMG risk factor on 
+an investment universe of &lt;2000 stocks through the traditional Fama-French approach. Analyse this factor across different contexts, including temporally.
+Then, based on this analytical framework, produce optimisations to portfolio management. Including with regard to minimum variance portfolios and index reweighting. This will further the theme of not bearing unrewarded risk by integrating the further dimension of carbon risk.</t>
+  </si>
+  <si>
+    <t>Portfolio techniques portion is not 
+relevant to my work.
+The considerations from the evaluation of the risk-factor approach will be broadly applicable to my work.</t>
   </si>
 </sst>
 </file>
@@ -727,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58E4A02-4BAA-41E0-832C-5DABBFDCD6F8}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" zoomScale="181" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="L4" zoomScale="181" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -809,13 +816,13 @@
         <v>18</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>29</v>
@@ -848,49 +855,49 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="404" x14ac:dyDescent="0.15">
@@ -898,19 +905,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="H4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>50</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>